<commit_message>
fixed 2002, de dupe is good for test output (csv)
</commit_message>
<xml_diff>
--- a/output/Intermediate_2_2002.xlsx
+++ b/output/Intermediate_2_2002.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1981,15 +1981,15 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> - as percentages</t>
+          <t>English and Communication</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
+        <v>6429</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2004,11 +2004,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>English and Communication</t>
+          <t>French</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>6429</v>
+        <v>809</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2027,11 +2027,11 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>Gaelic (Learners)</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>809</v>
+        <v>29</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2050,11 +2050,11 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Gaelic (Learners)</t>
+          <t>Gaidhlig</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2073,11 +2073,11 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Gaidhlig</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7</v>
+        <v>340</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2096,11 +2096,11 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Italian</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>340</v>
+        <v>90</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2119,11 +2119,11 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Italian</t>
+          <t>Latin</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2142,11 +2142,11 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Latin</t>
+          <t>Spanish</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>24</v>
+        <v>366</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2165,11 +2165,11 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Spanish</t>
+          <t>Accounting and Finance</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2188,11 +2188,11 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Accounting and Finance</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>377</v>
+        <v>6113</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2211,11 +2211,11 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Biology</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>6113</v>
+        <v>2351</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2234,11 +2234,11 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Biology</t>
+          <t>Biotechnology</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>2351</v>
+        <v>48</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2257,11 +2257,11 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Biotechnology</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>48</v>
+        <v>678</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2280,11 +2280,11 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Geology</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>678</v>
+        <v>4</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2303,11 +2303,11 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Geology</t>
+          <t>Managing Environmental Resources</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2326,11 +2326,11 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Managing Environmental Resources</t>
+          <t>Physics</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>25</v>
+        <v>380</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2349,11 +2349,11 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Physics</t>
+          <t>Amenity Horticulture</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>380</v>
+        <v>11</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2372,11 +2372,11 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Amenity Horticulture</t>
+          <t>Fish Husbandry</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2395,11 +2395,11 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Fish Husbandry</t>
+          <t>Forestry Practice</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2418,11 +2418,11 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Forestry Practice</t>
+          <t>Investigating Fish Rearing Systems</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2441,7 +2441,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Investigating Fish Rearing Systems</t>
+          <t>Investigating the Natural Environment</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -2464,11 +2464,11 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Investigating the Natural Environment</t>
+          <t>Plant Propagation</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2487,11 +2487,11 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Plant Propagation</t>
+          <t>Classical Studies</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2510,11 +2510,11 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Classical Studies</t>
+          <t>Economics</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2533,11 +2533,11 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Economics</t>
+          <t>Geography</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>83</v>
+        <v>602</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2556,11 +2556,11 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Geography</t>
+          <t>History</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>602</v>
+        <v>922</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2579,11 +2579,11 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>History</t>
+          <t>Modern Studies</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>922</v>
+        <v>704</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2602,11 +2602,11 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Modern Studies</t>
+          <t>Philosophy</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>704</v>
+        <v>45</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2625,11 +2625,11 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Philosophy</t>
+          <t>Politics</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2648,11 +2648,11 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Politics</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2671,11 +2671,11 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Psychology</t>
+          <t>Religious, Moral and Philosophical Studies</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2694,11 +2694,11 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Religious, Moral and Philosophical Studies</t>
+          <t>Sociology</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>322</v>
+        <v>106</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -2717,11 +2717,11 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Sociology</t>
+          <t>Administration</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>106</v>
+        <v>2649</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -2740,11 +2740,11 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Administration</t>
+          <t>Business Management</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2649</v>
+        <v>740</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2763,11 +2763,11 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Business Management</t>
+          <t>Care</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>740</v>
+        <v>635</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -2786,11 +2786,11 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Care</t>
+          <t>Care Issues for Society</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>635</v>
+        <v>162</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -2809,11 +2809,11 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Care Issues for Society</t>
+          <t>Computing</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>162</v>
+        <v>603</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -2832,11 +2832,11 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Computing</t>
+          <t>Construction Craft Skills</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>603</v>
+        <v>0</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -2855,11 +2855,11 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Construction Craft Skills</t>
+          <t>Construction Industry Practice</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -2878,11 +2878,11 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Construction Industry Practice</t>
+          <t>Craft and Design</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -2901,11 +2901,11 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Craft and Design</t>
+          <t>Design</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>147</v>
+        <v>12</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -2924,11 +2924,11 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Design</t>
+          <t>Electronic and Electrical Fundamentals</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -2947,11 +2947,11 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Electronic and Electrical Fundamentals</t>
+          <t>Engineering Craft Skills</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -2970,11 +2970,11 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Engineering Craft Skills</t>
+          <t>Fabrication and Welding</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -2993,11 +2993,11 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Fabrication and Welding</t>
+          <t>Graphic Communication</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>2</v>
+        <v>253</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -3016,11 +3016,11 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Graphic Communication</t>
+          <t>Health and Safety in Care Settings</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>253</v>
+        <v>88</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3039,11 +3039,11 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Health and Safety in Care Settings</t>
+          <t>Home Economics - Fashion and Textile Technology</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3062,11 +3062,11 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Home Economics - Fashion and Textile Technology</t>
+          <t>Home Economics - Health and Food Technology</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>63</v>
+        <v>262</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -3085,11 +3085,11 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Home Economics - Health and Food Technology</t>
+          <t>Home Economics - Lifestyle and Consumer Technology</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>262</v>
+        <v>84</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -3108,11 +3108,11 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Home Economics - Lifestyle and Consumer Technology</t>
+          <t>Hospitality - General Operations</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -3131,11 +3131,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Hospitality - General Operations</t>
+          <t>Hospitality - Practical Cookery</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>151</v>
+        <v>1847</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -3154,11 +3154,11 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Hospitality - Practical Cookery</t>
+          <t>Hospitality - Professional Cookery</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>1847</v>
+        <v>133</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -3177,11 +3177,11 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Hospitality - Professional Cookery</t>
+          <t>Hospitality - Reception and Accommodation Operations</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -3200,11 +3200,11 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Hospitality - Reception and Accommodation Operations</t>
+          <t>Information Systems</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>6</v>
+        <v>1143</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -3223,11 +3223,11 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Information Systems</t>
+          <t>Personal and Social Education</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>1143</v>
+        <v>23</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -3246,11 +3246,11 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Personal and Social Education</t>
+          <t>Selling Overseas Tourist Destinations</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3269,11 +3269,11 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Selling Overseas Tourist Destinations</t>
+          <t>Technological Studies</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3292,11 +3292,11 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Technological Studies</t>
+          <t>Travel and Tourism</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>10</v>
+        <v>527</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -3315,11 +3315,11 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Travel and Tourism</t>
+          <t>Woodworking Skills</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>527</v>
+        <v>367</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3338,11 +3338,11 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Woodworking Skills</t>
+          <t>Art and Design</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>367</v>
+        <v>1147</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -3361,11 +3361,11 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Art and Design</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>1147</v>
+        <v>337</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3384,11 +3384,11 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Media Studies</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>337</v>
+        <v>261</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3407,11 +3407,11 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Media Studies</t>
+          <t>Music</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>261</v>
+        <v>479</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -3430,11 +3430,11 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Fitness and Exercise</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>479</v>
+        <v>9</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3453,11 +3453,11 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Fitness and Exercise</t>
+          <t>Leading Sports Activities</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3476,11 +3476,11 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Leading Sports Activities</t>
+          <t>Physical Education</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>1</v>
+        <v>389</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -3491,52 +3491,6 @@
         <v>2002</v>
       </c>
       <c r="E133" t="inlineStr">
-        <is>
-          <t>Intermediate_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>Physical Education</t>
-        </is>
-      </c>
-      <c r="B134" t="n">
-        <v>389</v>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D134" t="n">
-        <v>2002</v>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Intermediate_2</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - as percentages</t>
-        </is>
-      </c>
-      <c r="B135" t="n">
-        <v>1</v>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D135" t="n">
-        <v>2002</v>
-      </c>
-      <c r="E135" t="inlineStr">
         <is>
           <t>Intermediate_2</t>
         </is>

</xml_diff>